<commit_message>
add new function to add outcome feature
</commit_message>
<xml_diff>
--- a/Notes/WhizzPM.xlsx
+++ b/Notes/WhizzPM.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="TODO" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Description" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
   <si>
     <t>UI Database</t>
   </si>
@@ -37,13 +38,100 @@
   </si>
   <si>
     <t>victor.sheng@whizzeducation.com</t>
+  </si>
+  <si>
+    <t>lesson_type</t>
+  </si>
+  <si>
+    <t>tutor_ex</t>
+  </si>
+  <si>
+    <t>run_mode</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>tutor_pb</t>
+  </si>
+  <si>
+    <t>total_help</t>
+  </si>
+  <si>
+    <t>replay</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>&gt; 0</t>
+  </si>
+  <si>
+    <t>progressions</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>1. The run_mode j and b are not present in early history.</t>
+  </si>
+  <si>
+    <t>num_pass</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only 1 record is found </t>
+  </si>
+  <si>
+    <t>num_fail</t>
+  </si>
+  <si>
+    <t>num_static</t>
+  </si>
+  <si>
+    <t>num_back</t>
+  </si>
+  <si>
+    <t>num_replay</t>
+  </si>
+  <si>
+    <t>num_assess</t>
+  </si>
+  <si>
+    <t>num_attempt</t>
+  </si>
+  <si>
+    <t>num_forward</t>
+  </si>
+  <si>
+    <t>Remove SettingWithCopyWarning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +147,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -68,7 +164,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -76,14 +172,114 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -406,11 +602,345 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q1" sqref="N1:Q1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="D15:D22"/>
+    <mergeCell ref="E15:E23"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add new class FeatureCM to refactor code
</commit_message>
<xml_diff>
--- a/Notes/WhizzPM.xlsx
+++ b/Notes/WhizzPM.xlsx
@@ -14,7 +14,9 @@
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="TODO" sheetId="2" r:id="rId2"/>
-    <sheet name="Data Description" sheetId="3" r:id="rId3"/>
+    <sheet name="Features" sheetId="4" r:id="rId3"/>
+    <sheet name="FeaturesEngineering" sheetId="5" r:id="rId4"/>
+    <sheet name="Data Description" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
   <si>
     <t>UI Database</t>
   </si>
@@ -125,6 +127,298 @@
   </si>
   <si>
     <t>Remove SettingWithCopyWarning</t>
+  </si>
+  <si>
+    <t>Personal Info</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Usage time</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>[0, 1 Month]</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Categorical</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Time since last attempt</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>time_taken_complete
+time_taken_incomplete</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Number of attempts</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>&gt;= 0</t>
+  </si>
+  <si>
+    <t>Name in DataFrame</t>
+  </si>
+  <si>
+    <t>Generating Function</t>
+  </si>
+  <si>
+    <t>Feature.add_age</t>
+  </si>
+  <si>
+    <t>Feature.add_usageTime</t>
+  </si>
+  <si>
+    <t>Feature.add_outcome</t>
+  </si>
+  <si>
+    <t>Percentage of incomplete attemps (measured by number)</t>
+  </si>
+  <si>
+    <t>Percentage of incomplete attemps (measured by time spent)</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>[0, 100]</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Feature.add_progressions</t>
+  </si>
+  <si>
+    <t>Progression level</t>
+  </si>
+  <si>
+    <t>Progression increment</t>
+  </si>
+  <si>
+    <t>progressions_delta</t>
+  </si>
+  <si>
+    <t>Effective progression</t>
+  </si>
+  <si>
+    <t>One / second</t>
+  </si>
+  <si>
+    <t>Progression increment per unit time</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">One way to add slopes to the linear model on the binned data is to add the original feature back in. We can do:
+(1) Only add the original feature
+(2) Add the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>interaction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the original feature and the binned features, e.g., the product between the two</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We can add </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>polynomial</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> features, which yields smooth fit.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Categorical variables: Use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>one-hot-encoding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to break into several dummy variables</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In linear model, it is helpful to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bin / discretize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> continuous data into multiple features.
+Two processes:
+(1) Bin: group continuously-ranged values into N bins;
+(2) One-hot encoding: 1 feature is split into N features.</t>
+    </r>
+  </si>
+  <si>
+    <t>Univariate nonlinear transformation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Most models work best when each feature is loosely Gaussian distributed. Using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>log and exp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is a hacky but simple and efficient way to achieve this. If value 0 is present in the data X, then we can transform using log(X+1), for example.
+This makes no difference to tree-based model where only order of data matters, but may help modelling using linear models and neural network which are very tied to scale and distribution of each feature.</t>
+    </r>
+  </si>
+  <si>
+    <t>Univariate statistics: 
+Consider each feature individually to see if there is a statistically significant relationship between feature and the target. Then the features that are related with the highest confidence are selected.
+In the case of classification, this is also known as ANOVA.</t>
+  </si>
+  <si>
+    <t>Model-based feature selection:
+The supervised model that is used for features selection does not need to be the same model that is used for the final supervised modelling. Examples pf feature selection models:
+(1) Tree-based models: importance of features
+(2) Linear models: absolute values of coefficients
+(3) Linear models with L1 penalty learn sparse coefficients, which only use a small subset of features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iterative feature selection:
+(1) Start with no features and add features one by one until some stopping criterion is reached
+(2) Start with all features and remove features one by on until some stopping criterion is reached </t>
+  </si>
+  <si>
+    <t>Adding a feature does not force a machine learning algorithm to use it, augmenting the data with expert knowledge doesn't hurt</t>
+  </si>
+  <si>
+    <t>Feature selection</t>
   </si>
 </sst>
 </file>
@@ -238,19 +532,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -262,13 +550,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -279,6 +570,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -602,7 +906,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,10 +923,356 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="72.5546875" style="15" customWidth="1"/>
+    <col min="3" max="4" width="9.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="B4" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
+      <c r="B9" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:A9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q1" sqref="N1:Q1"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,158 +1289,158 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="D2" s="4"/>
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="F3" s="6" t="s">
+      <c r="D3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="F4" s="6" t="s">
+      <c r="D4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>0</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -803,11 +1453,11 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -815,118 +1465,118 @@
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="3"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="9"/>
-      <c r="E17" s="3"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="13"/>
+      <c r="B18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="3"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="9"/>
-      <c r="E19" s="3"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="9"/>
-      <c r="E20" s="3"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="9"/>
-      <c r="E21" s="3"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="3"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="4">
         <v>0</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
add functions to compute hardship; aggregate data over customer months to analyze distribution.
</commit_message>
<xml_diff>
--- a/Notes/WhizzPM.xlsx
+++ b/Notes/WhizzPM.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="TODO" sheetId="2" r:id="rId2"/>
-    <sheet name="Features" sheetId="4" r:id="rId3"/>
-    <sheet name="FeaturesEngineering" sheetId="5" r:id="rId4"/>
-    <sheet name="Data Description" sheetId="3" r:id="rId5"/>
+    <sheet name="MixtureModel" sheetId="6" r:id="rId3"/>
+    <sheet name="Features" sheetId="4" r:id="rId4"/>
+    <sheet name="FeaturesEngineering" sheetId="5" r:id="rId5"/>
+    <sheet name="Data Description" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="115">
   <si>
     <t>UI Database</t>
   </si>
@@ -186,10 +187,6 @@
     <t>age</t>
   </si>
   <si>
-    <t>time_taken_complete
-time_taken_incomplete</t>
-  </si>
-  <si>
     <t>Day</t>
   </si>
   <si>
@@ -232,9 +229,6 @@
     <t>%</t>
   </si>
   <si>
-    <t>[0, 100]</t>
-  </si>
-  <si>
     <t>Progress</t>
   </si>
   <si>
@@ -245,9 +239,6 @@
   </si>
   <si>
     <t>Progression increment</t>
-  </si>
-  <si>
-    <t>progressions_delta</t>
   </si>
   <si>
     <t>Effective progression</t>
@@ -419,6 +410,107 @@
   </si>
   <si>
     <t>Feature selection</t>
+  </si>
+  <si>
+    <t>Add a new field "churnable" to show if the customer is churnable next month</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>rate_assess
+rate_pass
+rate_fail
+rate_fwrd
+rate_back</t>
+  </si>
+  <si>
+    <t>usage_complete
+usage_incomplete
+usage</t>
+  </si>
+  <si>
+    <t>num_attempt
+num_complete
+num_incomplete</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>[0, 1]</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Feature.add_score</t>
+  </si>
+  <si>
+    <t>Feature.__init__</t>
+  </si>
+  <si>
+    <t>FeatureCM.add_age</t>
+  </si>
+  <si>
+    <t>FeatureCM._initialise</t>
+  </si>
+  <si>
+    <t>FeatureCM.add_usageTime</t>
+  </si>
+  <si>
+    <t>FeatureCM.add_outcome</t>
+  </si>
+  <si>
+    <t>FeatureCM.add_score</t>
+  </si>
+  <si>
+    <t>FeatureCM.add_progress</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>GaussianMixture</t>
+  </si>
+  <si>
+    <t>EM algorithm</t>
+  </si>
+  <si>
+    <t>Confidence ellipsoids</t>
+  </si>
+  <si>
+    <t>Baysian Information Criterion to assess the number of clusters</t>
+  </si>
+  <si>
+    <t>Option to constrain covariance shape - diagonal, spherical, etc.</t>
+  </si>
+  <si>
+    <t>The BIC criterion can be used to select the number of components in a Gaussian Mixture in an efficient way. In theory, it recovers the true number of components only in the asymptotic regime (i.e. if much data is available and assuming that the data was actually generated i.i.d. from a mixture of Gaussian distribution</t>
+  </si>
+  <si>
+    <t>There are unsolved data issues.</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>rate_incomplete_num</t>
+  </si>
+  <si>
+    <t>rate_incomplete_usage</t>
+  </si>
+  <si>
+    <t>last_access</t>
+  </si>
+  <si>
+    <t>Chun will give me the mark data</t>
+  </si>
+  <si>
+    <t>stackDepth</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
   </si>
 </sst>
 </file>
@@ -532,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -552,6 +644,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -574,16 +679,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -903,10 +999,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,6 +1012,16 @@
         <v>32</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -923,62 +1029,115 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="52.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.109375" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.6640625" customWidth="1"/>
     <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
         <v>45</v>
@@ -993,14 +1152,17 @@
         <v>51</v>
       </c>
       <c r="I2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D3" t="s">
@@ -1010,15 +1172,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
         <v>49</v>
@@ -1029,160 +1191,254 @@
       <c r="G4" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>52</v>
+      <c r="H4" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="I4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="J4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="8" t="s">
         <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
         <v>54</v>
       </c>
-      <c r="D6" t="s">
-        <v>55</v>
-      </c>
       <c r="E6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" t="s">
         <v>57</v>
-      </c>
-      <c r="F6" t="s">
-        <v>58</v>
       </c>
       <c r="G6" t="s">
         <v>41</v>
       </c>
-      <c r="H6" t="s">
-        <v>30</v>
+      <c r="H6" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="J6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>64</v>
+      <c r="B7" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
         <v>65</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
         <v>56</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>66</v>
       </c>
-      <c r="F8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="B10" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" t="s">
         <v>57</v>
-      </c>
-      <c r="F9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" t="s">
-        <v>58</v>
       </c>
       <c r="G10" t="s">
         <v>41</v>
       </c>
       <c r="H10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I10" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="I10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>75</v>
-      </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K13" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1191,7 +1447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B10"/>
   <sheetViews>
@@ -1201,62 +1457,62 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="72.5546875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="72.5546875" style="8" customWidth="1"/>
     <col min="3" max="4" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+    <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+    <row r="8" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
+      <c r="B8" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="15" t="s">
+    </row>
+    <row r="9" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="15" t="s">
+    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="15" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1267,12 +1523,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1286,9 +1542,11 @@
     <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1313,12 +1571,18 @@
       <c r="J1" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="L1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1337,10 +1601,16 @@
       <c r="J2" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+      <c r="L2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1357,10 +1627,16 @@
       <c r="J3" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14" t="s">
+      <c r="L3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1379,18 +1655,24 @@
       <c r="J4" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
+      <c r="L4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1398,9 +1680,9 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1408,8 +1690,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1420,8 +1702,8 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1430,7 +1712,7 @@
       </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1442,17 +1724,17 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
         <v>7</v>
@@ -1461,7 +1743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -1471,15 +1753,15 @@
       <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1488,30 +1770,30 @@
       <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
@@ -1523,11 +1805,11 @@
       <c r="C19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1536,19 +1818,19 @@
       <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
@@ -1560,8 +1842,8 @@
       <c r="C22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
@@ -1576,7 +1858,7 @@
       <c r="D23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="10"/>
+      <c r="E23" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
add simple ML analysis, especially decision tree for analysing importance of features
</commit_message>
<xml_diff>
--- a/Notes/WhizzPM.xlsx
+++ b/Notes/WhizzPM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="117">
   <si>
     <t>UI Database</t>
   </si>
@@ -511,6 +511,12 @@
   </si>
   <si>
     <t>1,2,3</t>
+  </si>
+  <si>
+    <t>progress_delta</t>
+  </si>
+  <si>
+    <t>Bin data: rate_assess, etc. --&gt; a continuous feature can be broken into a discrete/binary feature and a continuous feature</t>
   </si>
 </sst>
 </file>
@@ -655,6 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -679,7 +686,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -999,27 +1005,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="64.5546875" style="8" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1077,7 +1094,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1333,6 +1350,12 @@
       <c r="F9" t="s">
         <v>57</v>
       </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>100</v>
+      </c>
       <c r="I9" t="s">
         <v>67</v>
       </c>
@@ -1357,7 +1380,7 @@
         <v>41</v>
       </c>
       <c r="H10" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="I10" t="s">
         <v>67</v>
@@ -1491,7 +1514,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>83</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1499,13 +1522,13 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="8" t="s">
         <v>81</v>
       </c>
@@ -1527,7 +1550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -1579,10 +1602,10 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1609,8 +1632,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1635,8 +1658,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1658,21 +1681,21 @@
       <c r="L4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="20">
+      <c r="M4" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1681,8 +1704,8 @@
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1691,7 +1714,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="20" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1703,7 +1726,7 @@
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1753,15 +1776,15 @@
       <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1770,30 +1793,30 @@
       <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
@@ -1805,11 +1828,11 @@
       <c r="C19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="16"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1818,19 +1841,19 @@
       <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="16"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
@@ -1842,8 +1865,8 @@
       <c r="C22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="16"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
@@ -1858,7 +1881,7 @@
       <c r="D23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="15"/>
+      <c r="E23" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
tried more learning algorithms and sample analysis; refactor code;
</commit_message>
<xml_diff>
--- a/Notes/WhizzPM.xlsx
+++ b/Notes/WhizzPM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -577,15 +577,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -630,7 +621,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -662,25 +653,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1007,7 +995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1514,7 +1502,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>83</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1522,13 +1510,13 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="8" t="s">
         <v>81</v>
       </c>
@@ -1550,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1602,10 +1590,10 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1632,8 +1620,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1658,8 +1646,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1686,16 +1674,16 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1704,8 +1692,8 @@
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1714,7 +1702,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1726,7 +1714,7 @@
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1776,15 +1764,15 @@
       <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1793,30 +1781,30 @@
       <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
@@ -1828,11 +1816,11 @@
       <c r="C19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1841,19 +1829,19 @@
       <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
@@ -1865,8 +1853,8 @@
       <c r="C22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
@@ -1878,10 +1866,10 @@
       <c r="C23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="16"/>
+      <c r="E23" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
finish revise functions to add age and outcome to FeatureCM by accommodating inactive users
</commit_message>
<xml_diff>
--- a/Notes/WhizzPM.xlsx
+++ b/Notes/WhizzPM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="127">
   <si>
     <t>UI Database</t>
   </si>
@@ -517,6 +517,36 @@
   </si>
   <si>
     <t>Bin data: rate_assess, etc. --&gt; a continuous feature can be broken into a discrete/binary feature and a continuous feature</t>
+  </si>
+  <si>
+    <t>#The usage per customer month is decliing over time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># No activity --&gt; zero in the table, not missing information </t>
+  </si>
+  <si>
+    <t># math age calculation: take into account history info - low priority</t>
+  </si>
+  <si>
+    <t># pass and non-pass</t>
+  </si>
+  <si>
+    <t># pct of visits they are not in stack depth 1</t>
+  </si>
+  <si>
+    <t># time spent on stack depth 2 or 3</t>
+  </si>
+  <si>
+    <t># decline in usage time from previous customer month</t>
+  </si>
+  <si>
+    <t># 2 features about memories: (1)1/2 month subscribers, (2)length of past subscritions</t>
+  </si>
+  <si>
+    <t># Sequency of outcomes/incomplete/reply</t>
+  </si>
+  <si>
+    <t># Spending a more time for reply, not for tutors (new lessons), may be afraid of the new lesson difficulties.</t>
   </si>
 </sst>
 </file>
@@ -662,6 +692,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -669,9 +702,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -993,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1021,10 +1051,66 @@
       <c r="A5" s="8" t="s">
         <v>112</v>
       </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1538,7 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1590,10 +1676,10 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1620,8 +1706,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1646,8 +1732,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1674,16 +1760,16 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1692,8 +1778,8 @@
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1702,7 +1788,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1714,7 +1800,7 @@
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1764,15 +1850,15 @@
       <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1781,30 +1867,30 @@
       <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
@@ -1816,8 +1902,8 @@
       <c r="C19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
@@ -1829,8 +1915,8 @@
       <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
@@ -1840,8 +1926,8 @@
       <c r="C21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
@@ -1853,8 +1939,8 @@
       <c r="C22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
@@ -1869,7 +1955,7 @@
       <c r="D23" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="19"/>
+      <c r="E23" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
finish revising add_mark function
</commit_message>
<xml_diff>
--- a/Notes/WhizzPM.xlsx
+++ b/Notes/WhizzPM.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="127">
   <si>
     <t>UI Database</t>
   </si>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,11 +1087,17 @@
       <c r="A13" s="8" t="s">
         <v>121</v>
       </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>122</v>
       </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
@@ -1108,7 +1114,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
test the new code and fix previous notebook analysis
</commit_message>
<xml_diff>
--- a/Notes/WhizzPM.xlsx
+++ b/Notes/WhizzPM.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="127">
   <si>
     <t>UI Database</t>
   </si>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,6 +1068,9 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>118</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
finish the grouping analysis
</commit_message>
<xml_diff>
--- a/Notes/WhizzPM.xlsx
+++ b/Notes/WhizzPM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Features" sheetId="4" r:id="rId4"/>
     <sheet name="FeaturesEngineering" sheetId="5" r:id="rId5"/>
     <sheet name="Data Description" sheetId="3" r:id="rId6"/>
+    <sheet name="Grouping" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="139">
   <si>
     <t>UI Database</t>
   </si>
@@ -547,6 +548,42 @@
   </si>
   <si>
     <t># Spending a more time for reply, not for tutors (new lessons), may be afraid of the new lesson difficulties.</t>
+  </si>
+  <si>
+    <t>Group No.</t>
+  </si>
+  <si>
+    <t>Inactive subscribers</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Mask</t>
+  </si>
+  <si>
+    <t>df_whizz1.active==0</t>
+  </si>
+  <si>
+    <t>Active subscribers taking no assessment</t>
+  </si>
+  <si>
+    <t>(df_whizz1.active==1) &amp; (df_whizz1.assess==0)</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>No lesson activity records.</t>
+  </si>
+  <si>
+    <t>No performance measure/ academic feedback from Whizz system.</t>
+  </si>
+  <si>
+    <t>Other active subscribers</t>
+  </si>
+  <si>
+    <t>(df_whizz1.active==1) &amp; (df_whizz1.assess==1)</t>
   </si>
 </sst>
 </file>
@@ -1025,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1981,4 +2018,77 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>